<commit_message>
Taking Osceola County out of Florida List
</commit_message>
<xml_diff>
--- a/rules/rules_states.xlsx
+++ b/rules/rules_states.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjohnson\Distributor Repo\sti-rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjohnson\Distributor Repo\sti-rules\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694A0A30-638B-4EC3-9B04-46B88C087CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A04482-9E97-4C15-841E-C5EBD508FC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3200,6 +3200,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D87BAF-62BF-47AE-BAA7-83BF92949FF0}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
@@ -3500,6 +3501,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF60086F-4E23-4552-812A-D6F349AB4AAA}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3579,6 +3581,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090E2328-4252-44D7-8F9F-0FEE326AAA47}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3843,6 +3846,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E0E31F-B62D-4680-B1F4-A49EBE3A95E3}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3896,6 +3900,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D06277F-CA4D-4882-884C-94F8DEB12FD8}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3958,6 +3963,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AABC6B03-4CD4-438B-B773-90767DEF6D87}">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4215,6 +4221,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8813E460-3269-433D-A176-13509591D858}">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:G769"/>
   <sheetViews>
     <sheetView topLeftCell="A565" workbookViewId="0">
@@ -15011,6 +15018,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A62CCD-58B9-4103-88C1-CBBD2D162002}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15105,10 +15113,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E97AF7-D224-4CB4-A89E-0B3789B9F7F6}">
-  <dimension ref="A1:G68"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15120,7 +15129,7 @@
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -15140,7 +15149,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>504</v>
       </c>
@@ -15154,7 +15163,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>339</v>
       </c>
@@ -15167,8 +15176,20 @@
       <c r="E3" t="s">
         <v>822</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>536</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>598</v>
+      </c>
+      <c r="L3" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>505</v>
       </c>
@@ -15182,7 +15203,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>506</v>
       </c>
@@ -15196,7 +15217,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>507</v>
       </c>
@@ -15210,7 +15231,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>508</v>
       </c>
@@ -15224,7 +15245,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -15238,7 +15259,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>509</v>
       </c>
@@ -15252,7 +15273,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>510</v>
       </c>
@@ -15266,7 +15287,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -15280,7 +15301,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>511</v>
       </c>
@@ -15294,7 +15315,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>239</v>
       </c>
@@ -15308,7 +15329,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>512</v>
       </c>
@@ -15322,7 +15343,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>513</v>
       </c>
@@ -15336,7 +15357,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>514</v>
       </c>
@@ -15814,13 +15835,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B50" t="s">
         <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>598</v>
+        <v>837</v>
       </c>
       <c r="E50" t="s">
         <v>822</v>
@@ -15828,13 +15849,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B51" t="s">
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>837</v>
+        <v>599</v>
       </c>
       <c r="E51" t="s">
         <v>822</v>
@@ -15842,13 +15863,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B52" t="s">
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="E52" t="s">
         <v>822</v>
@@ -15856,13 +15877,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>539</v>
+        <v>356</v>
       </c>
       <c r="B53" t="s">
         <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>600</v>
+        <v>574</v>
       </c>
       <c r="E53" t="s">
         <v>822</v>
@@ -15870,13 +15891,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>356</v>
+        <v>138</v>
       </c>
       <c r="B54" t="s">
         <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>574</v>
+        <v>601</v>
       </c>
       <c r="E54" t="s">
         <v>822</v>
@@ -15884,13 +15905,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>138</v>
+        <v>540</v>
       </c>
       <c r="B55" t="s">
         <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="E55" t="s">
         <v>822</v>
@@ -15898,13 +15919,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B56" t="s">
         <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="E56" t="s">
         <v>822</v>
@@ -15912,13 +15933,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B57" t="s">
         <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="E57" t="s">
         <v>822</v>
@@ -15926,13 +15947,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B58" t="s">
         <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="E58" t="s">
         <v>822</v>
@@ -15940,13 +15961,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B59" t="s">
         <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="E59" t="s">
         <v>822</v>
@@ -15954,13 +15975,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B60" t="s">
         <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E60" t="s">
         <v>822</v>
@@ -15968,13 +15989,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B61" t="s">
         <v>2</v>
       </c>
       <c r="C61" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="E61" t="s">
         <v>822</v>
@@ -15982,13 +16003,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B62" t="s">
         <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="E62" t="s">
         <v>822</v>
@@ -15996,13 +16017,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>547</v>
+        <v>161</v>
       </c>
       <c r="B63" t="s">
         <v>2</v>
       </c>
       <c r="C63" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="E63" t="s">
         <v>822</v>
@@ -16010,13 +16031,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>161</v>
+        <v>548</v>
       </c>
       <c r="B64" t="s">
         <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E64" t="s">
         <v>822</v>
@@ -16024,13 +16045,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B65" t="s">
         <v>2</v>
       </c>
       <c r="C65" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="E65" t="s">
         <v>822</v>
@@ -16038,13 +16059,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B66" t="s">
         <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="E66" t="s">
         <v>822</v>
@@ -16052,29 +16073,15 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>550</v>
+        <v>176</v>
       </c>
       <c r="B67" t="s">
         <v>2</v>
       </c>
       <c r="C67" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="E67" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>176</v>
-      </c>
-      <c r="B68" t="s">
-        <v>2</v>
-      </c>
-      <c r="C68" t="s">
-        <v>614</v>
-      </c>
-      <c r="E68" t="s">
         <v>822</v>
       </c>
     </row>
@@ -16085,6 +16092,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0120148-02B5-41A0-B534-E70620D50CDF}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16171,6 +16179,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G103"/>
   <sheetViews>
     <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
@@ -17640,6 +17649,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A423D28C-3242-4F17-BAFA-5D15DE2DACDA}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17714,6 +17724,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3763F8-F71B-49F5-BE31-3104EC77150F}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17786,6 +17797,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E50632D9-A68B-45AC-B2E8-6A44F2626A3B}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
@@ -18999,6 +19011,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3485B542-A7AE-49A8-9570-1F6A41EC410A}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Changed Lee County number under NC
</commit_message>
<xml_diff>
--- a/rules/rules_states.xlsx
+++ b/rules/rules_states.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjohnson\Distributor Repo\sti-rules\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A04482-9E97-4C15-841E-C5EBD508FC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7FAAA-8E25-425A-9320-ABED07942A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidelines" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4490" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4491" uniqueCount="839">
   <si>
     <t>sti</t>
   </si>
@@ -2832,6 +2832,9 @@
   </si>
   <si>
     <t>561-840-0148</t>
+  </si>
+  <si>
+    <t>919-718-4632</t>
   </si>
 </sst>
 </file>
@@ -15116,8 +15119,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16182,8 +16185,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17800,8 +17803,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18464,6 +18467,9 @@
       </c>
       <c r="B54" t="s">
         <v>817</v>
+      </c>
+      <c r="C54" t="s">
+        <v>838</v>
       </c>
       <c r="E54" t="s">
         <v>291</v>

</xml_diff>